<commit_message>
Electrolyser Data Updated(name of the sheet) and excel reader adapted for electrolyser. Now 2 libraries arrives at technical comparison
</commit_message>
<xml_diff>
--- a/Electrolyser data.xlsx
+++ b/Electrolyser data.xlsx
@@ -5,16 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aaltofi.sharepoint.com/sites/AEPCoursestudentproject2024-VTTProject2/Shared Documents/VTT Project 2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matis\Desktop\Aalto S1\Advanced Energy Project\SMR-X-H2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="431" documentId="11_73D32B72FC33B3B87482EAA6969955EA1A9E5F3A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{44A1E5D7-F0DD-4FC5-B681-68CBD01CEA6B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D87AB419-E433-4B1C-97F1-FFE0C0DDF2F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Script (Main)" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -460,9 +460,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -474,6 +471,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -815,7 +815,7 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="43.44140625" customWidth="1"/>
     <col min="2" max="2" width="25.5546875" customWidth="1"/>
@@ -840,16 +840,16 @@
       <c r="E1" s="4"/>
     </row>
     <row r="2" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E2" s="2" t="s">
@@ -857,10 +857,10 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
+      <c r="A3" s="9"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
       <c r="E3" s="2" t="s">
         <v>9</v>
       </c>
@@ -985,16 +985,16 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="9" t="s">
         <v>42</v>
       </c>
       <c r="E11" s="2" t="s">
@@ -1002,10 +1002,10 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
+      <c r="A12" s="9"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
       <c r="E12" s="2" t="s">
         <v>44</v>
       </c>
@@ -1045,28 +1045,28 @@
       </c>
     </row>
     <row r="15" spans="1:5" ht="57.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="E15" s="9" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
+      <c r="A16" s="9"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
@@ -1089,6 +1089,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="C11:C12"/>
@@ -1097,11 +1102,6 @@
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="D2:D3"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1112,10 +1112,10 @@
   <dimension ref="A1:AD6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
@@ -1143,551 +1143,551 @@
     <col min="29" max="30" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="9" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:30" s="8" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="M1" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="N1" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="O1" s="8" t="s">
+      <c r="O1" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="P1" s="8" t="s">
+      <c r="P1" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="Q1" s="8" t="s">
+      <c r="Q1" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="R1" s="8" t="s">
+      <c r="R1" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="8" t="s">
+      <c r="S1" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="8" t="s">
+      <c r="T1" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="U1" s="8" t="s">
+      <c r="U1" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="V1" s="8" t="s">
+      <c r="V1" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="W1" s="8" t="s">
+      <c r="W1" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="X1" s="8" t="s">
+      <c r="X1" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="Y1" s="8" t="s">
+      <c r="Y1" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="Z1" s="8" t="s">
+      <c r="Z1" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="AA1" s="8" t="s">
+      <c r="AA1" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="AB1" s="8" t="s">
+      <c r="AB1" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="AC1" s="8" t="s">
+      <c r="AC1" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="AD1" s="8" t="s">
+      <c r="AD1" s="7" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A2" s="7">
+      <c r="A2" s="6">
         <v>0</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="K2" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="L2" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="M2" s="7" t="s">
+      <c r="M2" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="N2" s="7" t="s">
+      <c r="N2" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="O2" s="7" t="s">
+      <c r="O2" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="P2" s="7" t="s">
+      <c r="P2" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="Q2" s="7" t="s">
+      <c r="Q2" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="R2" s="7" t="s">
+      <c r="R2" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="S2" s="7" t="s">
+      <c r="S2" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="T2" s="7" t="s">
+      <c r="T2" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="U2" s="7" t="s">
+      <c r="U2" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="V2" s="7" t="s">
+      <c r="V2" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="W2" s="7" t="s">
+      <c r="W2" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="X2" s="7" t="s">
+      <c r="X2" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="Y2" s="7" t="s">
+      <c r="Y2" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="Z2" s="7" t="s">
+      <c r="Z2" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="AA2" s="7" t="s">
+      <c r="AA2" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="AB2" s="7" t="s">
+      <c r="AB2" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="AC2" s="7" t="s">
+      <c r="AC2" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="AD2" s="7" t="s">
+      <c r="AD2" s="6" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="5">
         <v>70</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="5">
         <v>90</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="5">
         <v>30</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="5">
         <v>0.4</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="5">
         <v>1</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G3" s="5">
         <v>50</v>
       </c>
-      <c r="H3" s="6">
+      <c r="H3" s="5">
         <v>78</v>
       </c>
-      <c r="I3" s="6">
+      <c r="I3" s="5">
         <v>270</v>
       </c>
-      <c r="J3" s="6">
+      <c r="J3" s="5">
         <v>450</v>
       </c>
-      <c r="K3" s="6">
+      <c r="K3" s="5">
         <v>800</v>
       </c>
-      <c r="L3" s="6">
+      <c r="L3" s="5">
         <v>1500</v>
       </c>
-      <c r="M3" s="6">
+      <c r="M3" s="5">
         <v>60000</v>
       </c>
-      <c r="N3" s="6">
+      <c r="N3" s="5">
         <v>100000</v>
       </c>
-      <c r="O3" s="6">
+      <c r="O3" s="5">
         <v>0.13</v>
       </c>
-      <c r="P3" s="6">
+      <c r="P3" s="5">
         <v>1</v>
       </c>
-      <c r="Q3" s="6">
+      <c r="Q3" s="5">
         <v>30</v>
       </c>
-      <c r="R3" s="6">
+      <c r="R3" s="5">
         <v>10</v>
       </c>
-      <c r="S3" s="6">
+      <c r="S3" s="5">
         <v>40</v>
       </c>
-      <c r="T3" s="6">
+      <c r="T3" s="5">
         <v>46</v>
       </c>
-      <c r="U3" s="6">
+      <c r="U3" s="5">
         <v>70</v>
       </c>
-      <c r="V3" s="6">
+      <c r="V3" s="5">
         <v>70</v>
       </c>
-      <c r="W3" s="6">
+      <c r="W3" s="5">
         <v>90</v>
       </c>
-      <c r="X3" s="6">
+      <c r="X3" s="5">
         <v>1</v>
       </c>
-      <c r="Y3" s="6">
+      <c r="Y3" s="5">
         <v>30</v>
       </c>
-      <c r="Z3" s="6">
+      <c r="Z3" s="5">
         <v>50</v>
       </c>
-      <c r="AA3" s="6">
+      <c r="AA3" s="5">
         <v>6</v>
       </c>
-      <c r="AB3" s="6">
+      <c r="AB3" s="5">
         <v>80</v>
       </c>
-      <c r="AC3" s="6">
+      <c r="AC3" s="5">
         <v>580</v>
       </c>
-      <c r="AD3" s="6">
+      <c r="AD3" s="5">
         <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="5">
         <v>40</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="5">
         <v>80</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="5">
         <v>35</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="5">
         <v>0.2</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="5">
         <v>4</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="5">
         <v>57</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="5">
         <v>69</v>
       </c>
-      <c r="I4" s="6">
+      <c r="I4" s="5">
         <v>200</v>
       </c>
-      <c r="J4" s="6">
+      <c r="J4" s="5">
         <v>200</v>
       </c>
-      <c r="K4" s="6">
+      <c r="K4" s="5">
         <v>3333</v>
       </c>
-      <c r="L4" s="6">
+      <c r="L4" s="5">
         <v>3333</v>
       </c>
-      <c r="M4" s="6">
+      <c r="M4" s="5">
         <v>5000</v>
       </c>
-      <c r="N4" s="6">
+      <c r="N4" s="5">
         <v>40000</v>
       </c>
-      <c r="O4" s="6">
+      <c r="O4" s="5">
         <v>0.4</v>
       </c>
-      <c r="P4" s="6">
+      <c r="P4" s="5">
         <v>30</v>
       </c>
-      <c r="Q4" s="6">
+      <c r="Q4" s="5">
         <v>20</v>
       </c>
-      <c r="R4" s="6">
+      <c r="R4" s="5">
         <v>10</v>
       </c>
-      <c r="S4" s="6">
+      <c r="S4" s="5">
         <v>20</v>
       </c>
-      <c r="T4" s="6">
+      <c r="T4" s="5">
         <v>55</v>
       </c>
-      <c r="U4" s="6">
+      <c r="U4" s="5">
         <v>60</v>
       </c>
-      <c r="V4" s="6">
+      <c r="V4" s="5">
         <v>50</v>
       </c>
-      <c r="W4" s="6">
+      <c r="W4" s="5">
         <v>60</v>
       </c>
-      <c r="X4" s="6">
+      <c r="X4" s="5">
         <v>1</v>
       </c>
-      <c r="Y4" s="6">
+      <c r="Y4" s="5">
         <v>30</v>
       </c>
-      <c r="Z4" s="6">
+      <c r="Z4" s="5">
         <v>30</v>
       </c>
-      <c r="AA4" s="6">
+      <c r="AA4" s="5">
         <v>2</v>
       </c>
-      <c r="AB4" s="6">
+      <c r="AB4" s="5">
         <v>50</v>
       </c>
-      <c r="AC4" s="6"/>
-      <c r="AD4" s="6"/>
+      <c r="AC4" s="5"/>
+      <c r="AD4" s="5"/>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="5">
         <v>50</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="5">
         <v>80</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="5">
         <v>80</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="5">
         <v>0.2</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="5">
         <v>2</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="5">
         <v>50</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="5">
         <v>83</v>
       </c>
-      <c r="I5" s="6">
+      <c r="I5" s="5">
         <v>400</v>
       </c>
-      <c r="J5" s="6">
+      <c r="J5" s="5">
         <v>870</v>
       </c>
-      <c r="K5" s="6">
+      <c r="K5" s="5">
         <v>1400</v>
       </c>
-      <c r="L5" s="6">
+      <c r="L5" s="5">
         <v>2100</v>
       </c>
-      <c r="M5" s="6">
+      <c r="M5" s="5">
         <v>50000</v>
       </c>
-      <c r="N5" s="6">
+      <c r="N5" s="5">
         <v>90000</v>
       </c>
-      <c r="O5" s="6">
+      <c r="O5" s="5">
         <v>0.25</v>
       </c>
-      <c r="P5" s="6">
+      <c r="P5" s="5">
         <v>0.16666600000000001</v>
       </c>
-      <c r="Q5" s="6">
+      <c r="Q5" s="5">
         <v>5</v>
       </c>
-      <c r="R5" s="6">
+      <c r="R5" s="5">
         <v>5</v>
       </c>
-      <c r="S5" s="6">
+      <c r="S5" s="5">
         <v>10</v>
       </c>
-      <c r="T5" s="6">
+      <c r="T5" s="5">
         <v>55</v>
       </c>
-      <c r="U5" s="6">
+      <c r="U5" s="5">
         <v>60</v>
       </c>
-      <c r="V5" s="6">
+      <c r="V5" s="5">
         <v>50</v>
       </c>
-      <c r="W5" s="6">
+      <c r="W5" s="5">
         <v>80</v>
       </c>
-      <c r="X5" s="6">
+      <c r="X5" s="5">
         <v>30</v>
       </c>
-      <c r="Y5" s="6">
+      <c r="Y5" s="5">
         <v>30</v>
       </c>
-      <c r="Z5" s="6">
+      <c r="Z5" s="5">
         <v>15</v>
       </c>
-      <c r="AA5" s="6">
+      <c r="AA5" s="5">
         <v>2</v>
       </c>
-      <c r="AB5" s="6">
+      <c r="AB5" s="5">
         <v>50</v>
       </c>
-      <c r="AC5" s="6">
+      <c r="AC5" s="5">
         <v>760</v>
       </c>
-      <c r="AD5" s="6">
+      <c r="AD5" s="5">
         <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="5">
         <v>500</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="5">
         <v>900</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="5">
         <v>2</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="5">
         <v>0.5</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="5">
         <v>1.5</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="5">
         <v>38</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H6" s="5">
         <v>48</v>
       </c>
-      <c r="I6" s="6">
+      <c r="I6" s="5">
         <v>250</v>
       </c>
-      <c r="J6" s="6">
+      <c r="J6" s="5">
         <v>2000</v>
       </c>
-      <c r="K6" s="6">
+      <c r="K6" s="5">
         <v>917</v>
       </c>
-      <c r="L6" s="6">
+      <c r="L6" s="5">
         <v>4000</v>
       </c>
-      <c r="M6" s="6">
+      <c r="M6" s="5">
         <v>20000</v>
       </c>
-      <c r="N6" s="6">
+      <c r="N6" s="5">
         <v>50000</v>
       </c>
-      <c r="O6" s="6">
+      <c r="O6" s="5">
         <v>1</v>
       </c>
-      <c r="P6" s="6">
+      <c r="P6" s="5">
         <v>10</v>
       </c>
-      <c r="Q6" s="6">
+      <c r="Q6" s="5">
         <v>600</v>
       </c>
-      <c r="R6" s="6">
+      <c r="R6" s="5">
         <v>3</v>
       </c>
-      <c r="S6" s="6">
+      <c r="S6" s="5">
         <v>3</v>
       </c>
-      <c r="T6" s="6">
+      <c r="T6" s="5">
         <v>40</v>
       </c>
-      <c r="U6" s="6">
+      <c r="U6" s="5">
         <v>81</v>
       </c>
-      <c r="V6" s="6">
+      <c r="V6" s="5">
         <v>700</v>
       </c>
-      <c r="W6" s="6">
+      <c r="W6" s="5">
         <v>850</v>
       </c>
-      <c r="X6" s="6">
+      <c r="X6" s="5">
         <v>1</v>
       </c>
-      <c r="Y6" s="6">
+      <c r="Y6" s="5">
         <v>1</v>
       </c>
-      <c r="Z6" s="6">
+      <c r="Z6" s="5">
         <v>600</v>
       </c>
-      <c r="AA6" s="6">
+      <c r="AA6" s="5">
         <v>10</v>
       </c>
-      <c r="AB6" s="6">
+      <c r="AB6" s="5">
         <v>110</v>
       </c>
-      <c r="AC6" s="6">
+      <c r="AC6" s="5">
         <v>1000</v>
       </c>
-      <c r="AD6" s="6">
+      <c r="AD6" s="5">
         <v>250</v>
       </c>
     </row>
@@ -1697,16 +1697,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="56528f00-8daf-4285-8b2f-184ebce7f2e9">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EF98156A4E08ED42B22DA6C86624442E" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="11ba5f1833b47c39d11f9a0fc9ca5ad0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="56528f00-8daf-4285-8b2f-184ebce7f2e9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5b814f87d70368c36b985d9f62a71433" ns2:_="">
     <xsd:import namespace="56528f00-8daf-4285-8b2f-184ebce7f2e9"/>
@@ -1884,6 +1874,16 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="56528f00-8daf-4285-8b2f-184ebce7f2e9">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1894,22 +1894,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C747844-6093-4F1A-B800-1A4131821663}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="56528f00-8daf-4285-8b2f-184ebce7f2e9"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E04138F4-C2EC-45BF-818E-E97EF4C3AE40}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1927,6 +1911,22 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C747844-6093-4F1A-B800-1A4131821663}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="56528f00-8daf-4285-8b2f-184ebce7f2e9"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A3B776E9-5BDE-42CD-8357-70C76205F0A2}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Technological comparison Temperature difference comparison and electrical output as Criteria. Changed All excel to adapt Data. Added the Max Production Calculation
</commit_message>
<xml_diff>
--- a/Electrolyser data.xlsx
+++ b/Electrolyser data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matis\Desktop\Aalto S1\Advanced Energy Project\SMR-X-H2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D87AB419-E433-4B1C-97F1-FFE0C0DDF2F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F681B2AD-2612-40CA-82F8-DBB1135F84B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="109">
   <si>
     <t>Technology</t>
   </si>
@@ -358,6 +358,12 @@
   </si>
   <si>
     <t>Efficiency (LHV)</t>
+  </si>
+  <si>
+    <t>KWh/kg H2</t>
+  </si>
+  <si>
+    <t>System heat needed</t>
   </si>
 </sst>
 </file>
@@ -811,8 +817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1089,11 +1095,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="C11:C12"/>
@@ -1102,6 +1103,11 @@
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="D2:D3"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1109,10 +1115,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A03B1312-1625-4FD3-BECF-56DDACB845AB}">
-  <dimension ref="A1:AD6"/>
+  <dimension ref="A1:AE6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="Z1" workbookViewId="0">
+      <selection activeCell="AG5" sqref="AG5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1141,9 +1147,10 @@
     <col min="26" max="26" width="9.21875" customWidth="1"/>
     <col min="27" max="27" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="29" max="30" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="8" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:31" s="8" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1234,8 +1241,11 @@
       <c r="AD1" s="7" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE1" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
         <v>0</v>
       </c>
@@ -1326,8 +1336,11 @@
       <c r="AD2" s="6" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE2" s="6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
@@ -1418,8 +1431,11 @@
       <c r="AD3" s="5">
         <v>150</v>
       </c>
-    </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE3" s="5">
+        <v>7.3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
@@ -1506,8 +1522,11 @@
       </c>
       <c r="AC4" s="5"/>
       <c r="AD4" s="5"/>
-    </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE4" s="5">
+        <v>7.8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>2</v>
       </c>
@@ -1598,8 +1617,11 @@
       <c r="AD5" s="5">
         <v>150</v>
       </c>
-    </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE5" s="5">
+        <v>7.8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>68</v>
       </c>
@@ -1689,6 +1711,9 @@
       </c>
       <c r="AD6" s="5">
         <v>250</v>
+      </c>
+      <c r="AE6" s="5">
+        <v>7.4</v>
       </c>
     </row>
   </sheetData>
@@ -1697,6 +1722,25 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="56528f00-8daf-4285-8b2f-184ebce7f2e9">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EF98156A4E08ED42B22DA6C86624442E" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="11ba5f1833b47c39d11f9a0fc9ca5ad0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="56528f00-8daf-4285-8b2f-184ebce7f2e9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5b814f87d70368c36b985d9f62a71433" ns2:_="">
     <xsd:import namespace="56528f00-8daf-4285-8b2f-184ebce7f2e9"/>
@@ -1874,39 +1918,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="56528f00-8daf-4285-8b2f-184ebce7f2e9">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E04138F4-C2EC-45BF-818E-E97EF4C3AE40}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A3B776E9-5BDE-42CD-8357-70C76205F0A2}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="56528f00-8daf-4285-8b2f-184ebce7f2e9"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1928,9 +1943,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A3B776E9-5BDE-42CD-8357-70C76205F0A2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E04138F4-C2EC-45BF-818E-E97EF4C3AE40}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="56528f00-8daf-4285-8b2f-184ebce7f2e9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Ranking of combinations implemented
</commit_message>
<xml_diff>
--- a/Electrolyser data.xlsx
+++ b/Electrolyser data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matis\Desktop\Aalto S1\Advanced Energy Project\SMR-X-H2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4692FAAE-0F89-4A2A-9D1F-937E496090DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C26616E5-33B0-4745-B324-6C3417301CDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -460,7 +460,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -498,11 +498,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -528,6 +539,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1143,11 +1157,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="C11:C12"/>
@@ -1156,6 +1165,11 @@
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="D2:D3"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1165,8 +1179,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A03B1312-1625-4FD3-BECF-56DDACB845AB}">
   <dimension ref="A1:AT6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AD1" workbookViewId="0">
-      <selection activeCell="AN10" sqref="AN10"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="M59" sqref="M59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1582,6 +1596,51 @@
       <c r="AE3" s="5">
         <v>7.3</v>
       </c>
+      <c r="AF3" s="10">
+        <v>0</v>
+      </c>
+      <c r="AG3" s="10">
+        <v>0</v>
+      </c>
+      <c r="AH3" s="10">
+        <v>0</v>
+      </c>
+      <c r="AI3" s="10">
+        <v>0</v>
+      </c>
+      <c r="AJ3" s="10">
+        <v>0</v>
+      </c>
+      <c r="AK3" s="10">
+        <v>0</v>
+      </c>
+      <c r="AL3" s="10">
+        <v>0</v>
+      </c>
+      <c r="AM3" s="10">
+        <v>0</v>
+      </c>
+      <c r="AN3" s="10">
+        <v>0</v>
+      </c>
+      <c r="AO3" s="10">
+        <v>0</v>
+      </c>
+      <c r="AP3" s="10">
+        <v>0</v>
+      </c>
+      <c r="AQ3" s="10">
+        <v>0</v>
+      </c>
+      <c r="AR3" s="10">
+        <v>0</v>
+      </c>
+      <c r="AS3" s="10">
+        <v>0</v>
+      </c>
+      <c r="AT3" s="10">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
@@ -1673,6 +1732,51 @@
       <c r="AE4" s="5">
         <v>7.8</v>
       </c>
+      <c r="AF4" s="10">
+        <v>0</v>
+      </c>
+      <c r="AG4" s="10">
+        <v>0</v>
+      </c>
+      <c r="AH4" s="10">
+        <v>0</v>
+      </c>
+      <c r="AI4" s="10">
+        <v>0</v>
+      </c>
+      <c r="AJ4" s="10">
+        <v>0</v>
+      </c>
+      <c r="AK4" s="10">
+        <v>0</v>
+      </c>
+      <c r="AL4" s="10">
+        <v>0</v>
+      </c>
+      <c r="AM4" s="10">
+        <v>0</v>
+      </c>
+      <c r="AN4" s="10">
+        <v>0</v>
+      </c>
+      <c r="AO4" s="10">
+        <v>0</v>
+      </c>
+      <c r="AP4" s="10">
+        <v>0</v>
+      </c>
+      <c r="AQ4" s="10">
+        <v>0</v>
+      </c>
+      <c r="AR4" s="10">
+        <v>0</v>
+      </c>
+      <c r="AS4" s="10">
+        <v>0</v>
+      </c>
+      <c r="AT4" s="10">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
@@ -1768,6 +1872,51 @@
       <c r="AE5" s="5">
         <v>7.8</v>
       </c>
+      <c r="AF5" s="10">
+        <v>0</v>
+      </c>
+      <c r="AG5" s="10">
+        <v>0</v>
+      </c>
+      <c r="AH5" s="10">
+        <v>0</v>
+      </c>
+      <c r="AI5" s="10">
+        <v>0</v>
+      </c>
+      <c r="AJ5" s="10">
+        <v>0</v>
+      </c>
+      <c r="AK5" s="10">
+        <v>0</v>
+      </c>
+      <c r="AL5" s="10">
+        <v>0</v>
+      </c>
+      <c r="AM5" s="10">
+        <v>0</v>
+      </c>
+      <c r="AN5" s="10">
+        <v>0</v>
+      </c>
+      <c r="AO5" s="10">
+        <v>0</v>
+      </c>
+      <c r="AP5" s="10">
+        <v>0</v>
+      </c>
+      <c r="AQ5" s="10">
+        <v>0</v>
+      </c>
+      <c r="AR5" s="10">
+        <v>0</v>
+      </c>
+      <c r="AS5" s="10">
+        <v>0</v>
+      </c>
+      <c r="AT5" s="10">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
@@ -1862,6 +2011,51 @@
       </c>
       <c r="AE6" s="5">
         <v>7.4</v>
+      </c>
+      <c r="AF6" s="10">
+        <v>0</v>
+      </c>
+      <c r="AG6" s="10">
+        <v>0</v>
+      </c>
+      <c r="AH6" s="10">
+        <v>0</v>
+      </c>
+      <c r="AI6" s="10">
+        <v>0</v>
+      </c>
+      <c r="AJ6" s="10">
+        <v>0</v>
+      </c>
+      <c r="AK6" s="10">
+        <v>0</v>
+      </c>
+      <c r="AL6" s="10">
+        <v>0</v>
+      </c>
+      <c r="AM6" s="10">
+        <v>0</v>
+      </c>
+      <c r="AN6" s="10">
+        <v>0</v>
+      </c>
+      <c r="AO6" s="10">
+        <v>0</v>
+      </c>
+      <c r="AP6" s="10">
+        <v>0</v>
+      </c>
+      <c r="AQ6" s="10">
+        <v>0</v>
+      </c>
+      <c r="AR6" s="10">
+        <v>0</v>
+      </c>
+      <c r="AS6" s="10">
+        <v>0</v>
+      </c>
+      <c r="AT6" s="10">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2048,6 +2242,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="56528f00-8daf-4285-8b2f-184ebce7f2e9">
@@ -2055,15 +2258,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2085,6 +2279,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A3B776E9-5BDE-42CD-8357-70C76205F0A2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C747844-6093-4F1A-B800-1A4131821663}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
@@ -2098,12 +2300,4 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A3B776E9-5BDE-42CD-8357-70C76205F0A2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Change Excel Data and Update Criteria function
</commit_message>
<xml_diff>
--- a/Electrolyser data.xlsx
+++ b/Electrolyser data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matis\Desktop\Aalto S1\Advanced Energy Project\SMR-X-H2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47003B0E-B81A-40B3-AC7B-F33CB40F0578}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4A32BE2F-8E0B-466D-A302-C1E3FEF1EC37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3300" yWindow="3552" windowWidth="17112" windowHeight="8796" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-3275" yWindow="-9450" windowWidth="16945" windowHeight="8710" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -339,6 +339,9 @@
     <t>Minimum Load Max</t>
   </si>
   <si>
+    <t>System Electricity Consumption</t>
+  </si>
+  <si>
     <t>Efficiency (LHV)</t>
   </si>
   <si>
@@ -409,9 +412,6 @@
   </si>
   <si>
     <t>/10</t>
-  </si>
-  <si>
-    <t>System Electricity Consumption</t>
   </si>
 </sst>
 </file>
@@ -919,8 +919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U17"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:U5"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1450,6 +1450,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="C11:C12"/>
@@ -1458,11 +1463,6 @@
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="D2:D3"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1472,7 +1472,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A03B1312-1625-4FD3-BECF-56DDACB845AB}">
   <dimension ref="A1:AT6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="AN1" workbookViewId="0">
+      <selection activeCell="AT12" sqref="AT12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1574,10 +1576,10 @@
         <v>99</v>
       </c>
       <c r="T1" s="7" t="s">
-        <v>124</v>
+        <v>100</v>
       </c>
       <c r="U1" s="7" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="V1" s="7" t="s">
         <v>82</v>
@@ -1586,28 +1588,28 @@
         <v>83</v>
       </c>
       <c r="X1" s="7" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="Y1" s="7" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="Z1" s="7" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="AA1" s="7" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="AB1" s="7" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="AC1" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="AD1" s="7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AE1" s="7" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="AF1" s="7" t="s">
         <v>6</v>
@@ -1660,139 +1662,139 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D2" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="P2" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q2" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="R2" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="S2" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="T2" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="U2" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="V2" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="W2" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="X2" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y2" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="F2" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="O2" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="P2" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="Q2" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="R2" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="S2" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="T2" s="6" t="s">
+      <c r="Z2" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="AA2" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="AB2" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="AC2" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="AD2" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="AE2" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="U2" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="V2" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="W2" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="X2" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="Y2" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="Z2" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="AA2" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="AB2" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="AC2" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="AD2" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="AE2" s="6" t="s">
-        <v>117</v>
-      </c>
       <c r="AF2" s="6" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="AG2" s="6" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="AH2" s="6" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="AI2" s="6" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="AJ2" s="6" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="AK2" s="6" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="AL2" s="6" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="AM2" s="6" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="AN2" s="6">
         <v>10</v>
       </c>
       <c r="AO2" s="6" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="AP2" s="6" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="AQ2" s="6" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="AR2" s="6" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="AS2" s="6" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="AT2" s="6" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:46" ht="14.4" x14ac:dyDescent="0.3">
@@ -1893,10 +1895,10 @@
         <v>10</v>
       </c>
       <c r="AG3" s="12">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AH3" s="12">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AI3" s="12">
         <v>9</v>
@@ -1911,16 +1913,16 @@
         <v>8</v>
       </c>
       <c r="AM3" s="12">
+        <v>6</v>
+      </c>
+      <c r="AN3" s="12">
+        <v>5</v>
+      </c>
+      <c r="AO3" s="12">
         <v>8</v>
       </c>
-      <c r="AN3" s="12">
+      <c r="AP3" s="12">
         <v>7</v>
-      </c>
-      <c r="AO3" s="12">
-        <v>9</v>
-      </c>
-      <c r="AP3" s="12">
-        <v>8</v>
       </c>
       <c r="AQ3" s="12">
         <v>5</v>
@@ -1929,10 +1931,10 @@
         <v>9</v>
       </c>
       <c r="AS3" s="12">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="AT3" s="12">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:46" ht="14.4" x14ac:dyDescent="0.3">
@@ -2029,10 +2031,10 @@
         <v>7</v>
       </c>
       <c r="AG4" s="12">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="AH4" s="12">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AI4" s="12">
         <v>3</v>
@@ -2047,16 +2049,16 @@
         <v>7</v>
       </c>
       <c r="AM4" s="12">
+        <v>6</v>
+      </c>
+      <c r="AN4" s="12">
+        <v>7</v>
+      </c>
+      <c r="AO4" s="12">
+        <v>7</v>
+      </c>
+      <c r="AP4" s="12">
         <v>8</v>
-      </c>
-      <c r="AN4" s="12">
-        <v>9</v>
-      </c>
-      <c r="AO4" s="12">
-        <v>8</v>
-      </c>
-      <c r="AP4" s="12">
-        <v>9</v>
       </c>
       <c r="AQ4" s="12">
         <v>5</v>
@@ -2065,10 +2067,10 @@
         <v>7</v>
       </c>
       <c r="AS4" s="12">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="AT4" s="12">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:46" ht="14.4" x14ac:dyDescent="0.3">
@@ -2169,10 +2171,10 @@
         <v>3</v>
       </c>
       <c r="AG5" s="12">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="AH5" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AI5" s="2">
         <v>7</v>
@@ -2187,16 +2189,16 @@
         <v>5</v>
       </c>
       <c r="AM5" s="2">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="AN5" s="2">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="AO5" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AP5" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AQ5" s="2">
         <v>5</v>
@@ -2205,10 +2207,10 @@
         <v>1</v>
       </c>
       <c r="AS5" s="2">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="AT5" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:46" ht="14.4" x14ac:dyDescent="0.3">
@@ -2309,10 +2311,10 @@
         <v>1</v>
       </c>
       <c r="AG6" s="12">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AH6" s="12">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AI6" s="12">
         <v>4</v>
@@ -2327,16 +2329,16 @@
         <v>4</v>
       </c>
       <c r="AM6" s="12">
+        <v>5</v>
+      </c>
+      <c r="AN6" s="12">
         <v>7</v>
       </c>
-      <c r="AN6" s="12">
-        <v>9</v>
-      </c>
       <c r="AO6" s="12">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AP6" s="12">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AQ6" s="12">
         <v>5</v>
@@ -2345,10 +2347,10 @@
         <v>6</v>
       </c>
       <c r="AS6" s="12">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="AT6" s="12">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -2357,6 +2359,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EF98156A4E08ED42B22DA6C86624442E" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="11ba5f1833b47c39d11f9a0fc9ca5ad0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="56528f00-8daf-4285-8b2f-184ebce7f2e9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5b814f87d70368c36b985d9f62a71433" ns2:_="">
     <xsd:import namespace="56528f00-8daf-4285-8b2f-184ebce7f2e9"/>
@@ -2534,15 +2545,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -2554,6 +2556,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A3B776E9-5BDE-42CD-8357-70C76205F0A2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E04138F4-C2EC-45BF-818E-E97EF4C3AE40}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2571,20 +2581,18 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A3B776E9-5BDE-42CD-8357-70C76205F0A2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C747844-6093-4F1A-B800-1A4131821663}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="56528f00-8daf-4285-8b2f-184ebce7f2e9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="56528f00-8daf-4285-8b2f-184ebce7f2e9"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>